<commit_message>
dodano sprawozdanie z zadania 1
</commit_message>
<xml_diff>
--- a/QuickSort.xlsx
+++ b/QuickSort.xlsx
@@ -609,7 +609,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Optymistycznie</c:v>
+            <c:v>Pesymistyczny</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
@@ -734,7 +734,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Pesymistycznie</c:v>
+            <c:v>Optymistyczny</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
@@ -889,11 +889,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="176655360"/>
-        <c:axId val="176657152"/>
+        <c:axId val="177304704"/>
+        <c:axId val="177306624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="176655360"/>
+        <c:axId val="177304704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -906,17 +906,17 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1400"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL"/>
+                  <a:rPr lang="pl-PL" sz="1400"/>
                   <a:t>Ilość</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:rPr lang="pl-PL" sz="1400" baseline="0"/>
                   <a:t> danych w kolekcji</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" sz="1400"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -927,7 +927,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="176657152"/>
+        <c:crossAx val="177306624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -935,7 +935,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="176657152"/>
+        <c:axId val="177306624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -952,14 +952,14 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL"/>
+                  <a:rPr lang="pl-PL" sz="1400"/>
                   <a:t>Czas</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="pl-PL" baseline="0"/>
-                  <a:t> sortowania</a:t>
+                  <a:rPr lang="pl-PL" sz="1400" baseline="0"/>
+                  <a:t> sortowania [ms]</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" sz="1400"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -970,13 +970,39 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="176655360"/>
+        <c:crossAx val="177304704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="t"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -1009,10 +1035,10 @@
       <xdr:rowOff>114299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>114299</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1324,7 +1350,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+      <selection activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>